<commit_message>
added more part-names of symbols
</commit_message>
<xml_diff>
--- a/nanocopter-partlist.xlsx
+++ b/nanocopter-partlist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="-40" yWindow="-80" windowWidth="21600" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+  <si>
+    <t>Molex PicoBlade 8pin Stecker (für kabel)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Molex PicoBlade 8pin Sockel (rechtwinklig)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Si1958DH (Motor dual Mosfet)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAS3005B-02V (Motor Freilaufdiode)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>push-button</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PTS 525</t>
+  </si>
   <si>
     <t>Molex SlimStack 16pin (height 1.5mm) board-to-board receptacle</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -43,6 +66,82 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>Spezialteile</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NTC 10k</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NTCLE100E3103JB0</t>
+  </si>
+  <si>
+    <t>594-2381-640-63103</t>
+  </si>
+  <si>
+    <t>Fuse 3A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F0603G0R20FNTR</t>
+  </si>
+  <si>
+    <t>637-F0603FA3000V032</t>
+  </si>
+  <si>
+    <t>QTY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>15mOhm Shunt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WSLP0805R0150FEA</t>
+  </si>
+  <si>
+    <t>71-WSLP0805R0150FEA</t>
+  </si>
+  <si>
+    <t>Mosfets</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>78-SI1443EDH-T1-GE3</t>
+  </si>
+  <si>
+    <t>Si1443EDH (load switch)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SI1443EDH-T1-GE3</t>
+  </si>
+  <si>
+    <t>781-SI1958DH-T1-E3</t>
+  </si>
+  <si>
+    <t>SI1958DH-T1-E3</t>
+  </si>
+  <si>
+    <t>Diodes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAS 3005B-02V H6327</t>
+  </si>
+  <si>
+    <t>726-BAS3005B02VH6327</t>
+  </si>
+  <si>
+    <t>Molex PicoBlade 4pin Stecker (für Kabel)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Molex PicoBlade 4pin Sockel (rechtwinklig)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Beschreibung</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -75,10 +174,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Molex PicoBlade 8pin sockel (rechtwinklig)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>53261-0871</t>
   </si>
   <si>
@@ -107,10 +202,6 @@
   </si>
   <si>
     <t>538-50058-8000</t>
-  </si>
-  <si>
-    <t>Molex PicoBlade 8pin stecker (für kabel)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>54722-0164</t>
@@ -491,10 +582,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:K10"/>
+  <dimension ref="A2:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -502,12 +593,13 @@
     <col min="1" max="1" width="10.7109375" style="1"/>
     <col min="2" max="2" width="49.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" customWidth="1"/>
+    <col min="10" max="10" width="1.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -515,113 +607,265 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="I2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26">
+        <v>0.21</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
all parts & values defined
Todo: footprints
</commit_message>
<xml_diff>
--- a/nanocopter-partlist.xlsx
+++ b/nanocopter-partlist.xlsx
@@ -19,7 +19,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+  <si>
+    <t>C_IN 2.2uF Low ESR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>963-LMK212BJ225MG-T</t>
+  </si>
+  <si>
+    <t>LMK212BJ105MG-T</t>
+  </si>
+  <si>
+    <t>C_SW 1uF Low ESR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>963-LMK212BJ105MG-T</t>
+  </si>
+  <si>
+    <t>JMK107BJ475MA-T</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>963-JMK107BJ475MA-T</t>
+  </si>
+  <si>
+    <t>Inductors</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IFSC1111AZER100M01</t>
+  </si>
+  <si>
+    <t>70-IFSC1111AZER100M0</t>
+  </si>
+  <si>
+    <t>LQH32CN100K33L</t>
+  </si>
+  <si>
+    <t>81-LQH32CN100K33L</t>
+  </si>
+  <si>
+    <t>Sepic: 10uH Murata</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sepic: 10uH Vishay (alternative)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBC2518T100K</t>
+  </si>
+  <si>
+    <t>963-CBC2518T100K</t>
+  </si>
+  <si>
+    <t>Sepic: 10uH Taiyo Yuden (alternative 2) (KLEIN!)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MBR0520 (SEPIC, ChargePump out)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DCDC C_OUT &amp; STM32 Bypass 4.7uF Low ESR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ferrite</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BLM18KG331SN1D</t>
+  </si>
+  <si>
+    <t>Widerstände</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spannungsteiler Sepic: 110k 1%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CR0603-FX-1103GLF</t>
+  </si>
+  <si>
+    <t>Spannungsteiler Sepic: 180k 1%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CR0603-FX-1803ELF</t>
+  </si>
+  <si>
+    <t>TODO: Richtige molex buchsen (smd) suchen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Molex PicoBlade 8pin Stecker (für kabel)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -208,6 +303,33 @@
   </si>
   <si>
     <t>538-54722-0164</t>
+  </si>
+  <si>
+    <t>MBR0520LT1G</t>
+  </si>
+  <si>
+    <t>863-MBR0520LT1G</t>
+  </si>
+  <si>
+    <t>Capacitors</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sepic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JMK316BJ106ML-T</t>
+  </si>
+  <si>
+    <t>963-JMK316BJ106ML-T</t>
+  </si>
+  <si>
+    <t>C_OUT 10uF Low ESR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LMK212BJ225MG-T</t>
   </si>
 </sst>
 </file>
@@ -582,10 +704,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:L26"/>
+  <dimension ref="A2:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -612,85 +734,85 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="F7">
         <v>7.9</v>
@@ -698,63 +820,68 @@
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="B15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="F18">
         <v>0.35</v>
@@ -762,16 +889,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="B19" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="F19">
         <v>0.28000000000000003</v>
@@ -779,16 +906,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="B20" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="F20">
         <v>0.81</v>
@@ -796,10 +923,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="B21" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -807,19 +934,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="F23">
         <v>0.27</v>
@@ -827,16 +954,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="B24" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D24">
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F24">
         <v>0.7</v>
@@ -844,22 +971,214 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D26">
         <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="F26">
         <v>0.21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added all refdes and most resistor/capacitor footprints
</commit_message>
<xml_diff>
--- a/nanocopter-partlist.xlsx
+++ b/nanocopter-partlist.xlsx
@@ -19,7 +19,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="93">
+  <si>
+    <t>Molex PicoBlade 4pin Sockel (rechtwinklig, smd)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Molex PicoBlade 8pin Sockel (rechtwinklig, smd)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>538-53261-0471</t>
+  </si>
+  <si>
+    <t>1.44 (ab 10)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>51021-0400</t>
+  </si>
+  <si>
+    <t>0.38 (ab 10)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>538-51021-0400</t>
+  </si>
   <si>
     <t>C_IN 2.2uF Low ESR</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -112,18 +137,19 @@
     <t>CR0603-FX-1803ELF</t>
   </si>
   <si>
-    <t>TODO: Richtige molex buchsen (smd) suchen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>F0603HI3000V032T</t>
+  </si>
+  <si>
+    <t>637-F0603HI3000V032</t>
+  </si>
+  <si>
+    <t>53261-0471</t>
   </si>
   <si>
     <t>Molex PicoBlade 8pin Stecker (für kabel)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Molex PicoBlade 8pin Sockel (rechtwinklig)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Si1958DH (Motor dual Mosfet)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -179,12 +205,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>F0603G0R20FNTR</t>
-  </si>
-  <si>
-    <t>637-F0603FA3000V032</t>
-  </si>
-  <si>
     <t>QTY</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -230,10 +250,6 @@
   </si>
   <si>
     <t>Molex PicoBlade 4pin Stecker (für Kabel)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Molex PicoBlade 4pin Sockel (rechtwinklig)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -336,7 +352,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -348,6 +364,16 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="63"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -371,9 +397,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -706,8 +736,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A2:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -734,154 +764,173 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>69</v>
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" t="s">
-        <v>76</v>
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7">
-        <v>7.9</v>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="B10" t="s">
-        <v>59</v>
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9">
+        <v>7.9</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="B13" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="B15" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F18">
         <v>0.35</v>
@@ -889,33 +938,33 @@
     </row>
     <row r="19" spans="1:6">
       <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" t="s">
-        <v>45</v>
+      <c r="E19" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="F19">
-        <v>0.28000000000000003</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F20">
         <v>0.81</v>
@@ -923,10 +972,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="B21" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -934,19 +983,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F23">
         <v>0.27</v>
@@ -954,16 +1003,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="B24" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D24">
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F24">
         <v>0.7</v>
@@ -971,19 +1020,19 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D26">
         <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F26">
         <v>0.21</v>
@@ -991,16 +1040,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="B27" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F27">
         <v>0.35</v>
@@ -1008,24 +1057,24 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F31">
         <v>0.46</v>
@@ -1033,16 +1082,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="B32" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F32">
         <v>0.24</v>
@@ -1050,16 +1099,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="B33" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F33">
         <v>0.36</v>
@@ -1067,16 +1116,16 @@
     </row>
     <row r="35" spans="1:6">
       <c r="B35" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D35">
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F35">
         <v>0.27</v>
@@ -1084,19 +1133,19 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D37">
         <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F37">
         <v>0.53</v>
@@ -1104,16 +1153,16 @@
     </row>
     <row r="38" spans="1:6">
       <c r="B38" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D38">
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F38">
         <v>0.28999999999999998</v>
@@ -1121,16 +1170,16 @@
     </row>
     <row r="39" spans="1:6">
       <c r="B39" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F39">
         <v>0.17</v>
@@ -1138,19 +1187,19 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F41">
         <v>0.34</v>
@@ -1158,13 +1207,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B43" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1172,10 +1221,10 @@
     </row>
     <row r="44" spans="1:6">
       <c r="B44" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D44">
         <v>1</v>

</xml_diff>

<commit_message>
added possible usb-connector to partlist
</commit_message>
<xml_diff>
--- a/nanocopter-partlist.xlsx
+++ b/nanocopter-partlist.xlsx
@@ -19,7 +19,128 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
+  <si>
+    <t>SI1443EDH-T1-GE3</t>
+  </si>
+  <si>
+    <t>781-SI1958DH-T1-E3</t>
+  </si>
+  <si>
+    <t>SI1958DH-T1-E3</t>
+  </si>
+  <si>
+    <t>Diodes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAS 3005B-02V H6327</t>
+  </si>
+  <si>
+    <t>726-BAS3005B02VH6327</t>
+  </si>
+  <si>
+    <t>Molex PicoBlade 4pin Stecker (für Kabel)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mouser</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Preis</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Digikey</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Farnell</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kategorie</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stecker</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>53261-0871</t>
+  </si>
+  <si>
+    <t>538-53261-0871</t>
+  </si>
+  <si>
+    <t>1.81 (ab 10)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>51021-0800</t>
+  </si>
+  <si>
+    <t>538-51021-0800</t>
+  </si>
+  <si>
+    <t>0.38 (ab 10)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Molex PicoBlade pin crimps (100stk)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>50058-8000</t>
+  </si>
+  <si>
+    <t>538-50058-8000</t>
+  </si>
+  <si>
+    <t>54722-0164</t>
+  </si>
+  <si>
+    <t>538-54722-0164</t>
+  </si>
+  <si>
+    <t>MBR0520LT1G</t>
+  </si>
+  <si>
+    <t>863-MBR0520LT1G</t>
+  </si>
+  <si>
+    <t>Capacitors</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sepic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JMK316BJ106ML-T</t>
+  </si>
+  <si>
+    <t>963-JMK316BJ106ML-T</t>
+  </si>
+  <si>
+    <t>VJ0603D4R7CXPAJ</t>
+  </si>
+  <si>
+    <t>77-VJ0603D4R7CXPAJ</t>
+  </si>
+  <si>
+    <t>4.7pF 250V f. USB-Shield</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Molex PicoBlade 4pin Sockel (rechtwinklig, smd)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -246,117 +367,6 @@
   <si>
     <t>Si1443EDH (load switch)</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SI1443EDH-T1-GE3</t>
-  </si>
-  <si>
-    <t>781-SI1958DH-T1-E3</t>
-  </si>
-  <si>
-    <t>SI1958DH-T1-E3</t>
-  </si>
-  <si>
-    <t>Diodes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BAS 3005B-02V H6327</t>
-  </si>
-  <si>
-    <t>726-BAS3005B02VH6327</t>
-  </si>
-  <si>
-    <t>Molex PicoBlade 4pin Stecker (für Kabel)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Beschreibung</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mouser</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Preis</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Digikey</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Farnell</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kategorie</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stecker</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>53261-0871</t>
-  </si>
-  <si>
-    <t>538-53261-0871</t>
-  </si>
-  <si>
-    <t>1.81 (ab 10)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>51021-0800</t>
-  </si>
-  <si>
-    <t>538-51021-0800</t>
-  </si>
-  <si>
-    <t>0.38 (ab 10)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Molex PicoBlade pin crimps (100stk)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>50058-8000</t>
-  </si>
-  <si>
-    <t>538-50058-8000</t>
-  </si>
-  <si>
-    <t>54722-0164</t>
-  </si>
-  <si>
-    <t>538-54722-0164</t>
-  </si>
-  <si>
-    <t>MBR0520LT1G</t>
-  </si>
-  <si>
-    <t>863-MBR0520LT1G</t>
-  </si>
-  <si>
-    <t>Capacitors</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sepic</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>JMK316BJ106ML-T</t>
-  </si>
-  <si>
-    <t>963-JMK316BJ106ML-T</t>
   </si>
 </sst>
 </file>
@@ -748,7 +758,7 @@
   <dimension ref="A2:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -775,119 +785,119 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="B8" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="F9">
         <v>7.9</v>
@@ -895,53 +905,53 @@
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="B13" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="F18">
         <v>0.35</v>
@@ -949,16 +959,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="B19" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="F19">
         <v>0.32</v>
@@ -966,16 +976,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="B20" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="F20">
         <v>0.81</v>
@@ -983,10 +993,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="B21" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -994,19 +1004,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="F23">
         <v>0.27</v>
@@ -1014,16 +1024,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="B24" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="D24">
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="F24">
         <v>0.7</v>
@@ -1031,19 +1041,19 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="D26">
         <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="F26">
         <v>0.21</v>
@@ -1051,16 +1061,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="B27" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="F27">
         <v>0.35</v>
@@ -1068,24 +1078,24 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="F31">
         <v>0.46</v>
@@ -1093,16 +1103,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="B32" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D32">
         <v>3</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F32">
         <v>0.24</v>
@@ -1110,16 +1120,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="B33" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="F33">
         <v>0.17</v>
@@ -1127,16 +1137,16 @@
     </row>
     <row r="35" spans="1:6">
       <c r="B35" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="D35">
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="F35">
         <v>0.27</v>
@@ -1144,40 +1154,53 @@
     </row>
     <row r="36" spans="1:6">
       <c r="B36" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="F36">
         <v>0.09</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="C37" s="2"/>
-      <c r="E37" s="3"/>
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="F39">
         <v>0.53</v>
@@ -1185,16 +1208,16 @@
     </row>
     <row r="40" spans="1:6">
       <c r="B40" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D40">
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="F40">
         <v>0.28999999999999998</v>
@@ -1202,16 +1225,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="B41" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="D41">
         <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="F41">
         <v>0.17</v>
@@ -1219,19 +1242,19 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="F43">
         <v>0.34</v>
@@ -1239,13 +1262,13 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1253,10 +1276,10 @@
     </row>
     <row r="46" spans="1:6">
       <c r="B46" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1265,7 +1288,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>